<commit_message>
Adding mising fields for RTW report
</commit_message>
<xml_diff>
--- a/portfolio/CPR_Missing_Fields.xlsx
+++ b/portfolio/CPR_Missing_Fields.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="7635" windowHeight="4425"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="7635" windowHeight="4425" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Missing Fields" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="50">
   <si>
     <t>Mising field</t>
   </si>
@@ -429,6 +429,89 @@
     <t>Need 2 columns from 2 different tables:
 - Column DESCRIPTION from ANZSIC 
 - And column Tariff from ACTIVITY_DETAIL_AUDIT</t>
+  </si>
+  <si>
+    <t>Missing Field</t>
+  </si>
+  <si>
+    <t>EMICS table / columns</t>
+  </si>
+  <si>
+    <t>Missing fields of RTW Report</t>
+  </si>
+  <si>
+    <t>LT</t>
+  </si>
+  <si>
+    <t>WGT</t>
+  </si>
+  <si>
+    <t>Weeks_paid</t>
+  </si>
+  <si>
+    <t>Cert_Type</t>
+  </si>
+  <si>
+    <t>cost_code</t>
+  </si>
+  <si>
+    <t>cost_code2</t>
+  </si>
+  <si>
+    <t>calculated field</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Medical_Cert </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/ Type</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Payment_Recovery</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / wc_Hours &amp; wc_Minutes</t>
+    </r>
+  </si>
+  <si>
+    <t>Remuneration_Start</t>
+  </si>
+  <si>
+    <t>Remuneration_End</t>
+  </si>
+  <si>
+    <t>Measure_months</t>
   </si>
 </sst>
 </file>
@@ -487,7 +570,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -495,8 +578,32 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -801,9 +908,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:C1"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -814,11 +921,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -965,13 +1072,139 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+    <col min="2" max="2" width="42.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
seperate RTW from CPR
</commit_message>
<xml_diff>
--- a/portfolio/CPR_Missing_Fields.xlsx
+++ b/portfolio/CPR_Missing_Fields.xlsx
@@ -4,19 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="7635" windowHeight="4425" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="7635" windowHeight="4425"/>
   </bookViews>
   <sheets>
     <sheet name="Missing Fields" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Mising field</t>
   </si>
@@ -429,89 +428,6 @@
     <t>Need 2 columns from 2 different tables:
 - Column DESCRIPTION from ANZSIC 
 - And column Tariff from ACTIVITY_DETAIL_AUDIT</t>
-  </si>
-  <si>
-    <t>Missing Field</t>
-  </si>
-  <si>
-    <t>EMICS table / columns</t>
-  </si>
-  <si>
-    <t>Missing fields of RTW Report</t>
-  </si>
-  <si>
-    <t>LT</t>
-  </si>
-  <si>
-    <t>WGT</t>
-  </si>
-  <si>
-    <t>Weeks_paid</t>
-  </si>
-  <si>
-    <t>Cert_Type</t>
-  </si>
-  <si>
-    <t>cost_code</t>
-  </si>
-  <si>
-    <t>cost_code2</t>
-  </si>
-  <si>
-    <t>calculated field</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Medical_Cert </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>/ Type</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Payment_Recovery</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> / wc_Hours &amp; wc_Minutes</t>
-    </r>
-  </si>
-  <si>
-    <t>Remuneration_Start</t>
-  </si>
-  <si>
-    <t>Remuneration_End</t>
-  </si>
-  <si>
-    <t>Measure_months</t>
   </si>
 </sst>
 </file>
@@ -570,7 +486,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -578,32 +494,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -908,7 +800,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
@@ -921,11 +813,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1072,144 +964,6 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.5703125" customWidth="1"/>
-    <col min="2" max="2" width="42.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>